<commit_message>
gpa is now charted with box plots
</commit_message>
<xml_diff>
--- a/Group_Allocator.xlsx
+++ b/Group_Allocator.xlsx
@@ -9,27 +9,27 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10005" windowHeight="7905" tabRatio="870" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10005" windowHeight="7905" tabRatio="870"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="17" r:id="rId1"/>
     <sheet name="Student_Data" sheetId="3" r:id="rId2"/>
     <sheet name="Summary_Results" sheetId="7" r:id="rId3"/>
-    <sheet name="GPA_Chart" sheetId="530" r:id="rId4"/>
-    <sheet name="Gender_Chart" sheetId="531" r:id="rId5"/>
-    <sheet name="Civil_Chart" sheetId="532" r:id="rId6"/>
-    <sheet name="Electrical_Chart" sheetId="533" r:id="rId7"/>
-    <sheet name="CompSys_Chart" sheetId="534" r:id="rId8"/>
-    <sheet name="Software_Chart" sheetId="535" r:id="rId9"/>
-    <sheet name="Mechatronics_Chart" sheetId="536" r:id="rId10"/>
-    <sheet name="Chemmat_Chart" sheetId="537" r:id="rId11"/>
-    <sheet name="Mechanical_Chart" sheetId="538" r:id="rId12"/>
-    <sheet name="Biomedical_Chart" sheetId="539" r:id="rId13"/>
-    <sheet name="EngSci_Chart" sheetId="540" r:id="rId14"/>
-    <sheet name="European(E)_Chart" sheetId="541" r:id="rId15"/>
-    <sheet name="Pacific(E)_Chart" sheetId="542" r:id="rId16"/>
-    <sheet name="Indian(E)_Chart" sheetId="543" r:id="rId17"/>
-    <sheet name="Asian(E)_Chart" sheetId="544" r:id="rId18"/>
+    <sheet name="GPA_Chart" sheetId="605" r:id="rId4"/>
+    <sheet name="Gender_Chart" sheetId="606" r:id="rId5"/>
+    <sheet name="Civil_Chart" sheetId="607" r:id="rId6"/>
+    <sheet name="Electrical_Chart" sheetId="608" r:id="rId7"/>
+    <sheet name="CompSys_Chart" sheetId="609" r:id="rId8"/>
+    <sheet name="Software_Chart" sheetId="610" r:id="rId9"/>
+    <sheet name="Mechatronics_Chart" sheetId="611" r:id="rId10"/>
+    <sheet name="Chemmat_Chart" sheetId="612" r:id="rId11"/>
+    <sheet name="Mechanical_Chart" sheetId="613" r:id="rId12"/>
+    <sheet name="Biomedical_Chart" sheetId="614" r:id="rId13"/>
+    <sheet name="EngSci_Chart" sheetId="615" r:id="rId14"/>
+    <sheet name="European(E)_Chart" sheetId="616" r:id="rId15"/>
+    <sheet name="Pacific(E)_Chart" sheetId="617" r:id="rId16"/>
+    <sheet name="Indian(E)_Chart" sheetId="618" r:id="rId17"/>
+    <sheet name="Asian(E)_Chart" sheetId="619" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="ethnicity" localSheetId="1">OFFSET(Student_Data!$N$2,0,0,COUNTA(Student_Data!$A:$A)-1,1)</definedName>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2138" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="95">
   <si>
     <t>Specialisation</t>
   </si>
@@ -389,6 +389,36 @@
   </si>
   <si>
     <t>CompSys</t>
+  </si>
+  <si>
+    <t>gpa_min</t>
+  </si>
+  <si>
+    <t>gpa_q1</t>
+  </si>
+  <si>
+    <t>gpa_median</t>
+  </si>
+  <si>
+    <t>gpa_q3</t>
+  </si>
+  <si>
+    <t>gpa_max</t>
+  </si>
+  <si>
+    <t>gpa_d_min</t>
+  </si>
+  <si>
+    <t>gpa_d_q1</t>
+  </si>
+  <si>
+    <t>gpa_d_median</t>
+  </si>
+  <si>
+    <t>gpa_d_q3</t>
+  </si>
+  <si>
+    <t>gpa_d_max</t>
   </si>
 </sst>
 </file>
@@ -891,169 +921,156 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Mean GPA and Variance of GPA</a:t>
+              <a:t>GPA spread per group (lines bottom to top = Min, Q1, Median, Q3, Max)</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>GPA</c:v>
-          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:srgbClr val="5B9BD5"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:noFill/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Summary_Results!$A$3:$A$22</c:f>
+              <c:f>Summary_Results!$Z$3:$Z$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2.89</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>2.94</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>2.58</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>3.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>3.55</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>2.83</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>3.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>2.98</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>2.78</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>3.23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>3.56</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>2.31</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16</c:v>
+                  <c:v>3.08</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17</c:v>
+                  <c:v>2.74</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>2.56</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19</c:v>
+                  <c:v>3.23</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Summary_Results!$E$3:$E$22</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.05</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0599999999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.08</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.04</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.0599999999999996</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.0599999999999996</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.0199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.01</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5.1100000000000003</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.09</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5.0599999999999996</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.0599999999999996</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.04</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.03</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5.01</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.99</c:v>
+                  <c:v>3.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1062,144 +1079,410 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>GPA Variance</c:v>
-          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:srgbClr val="ED7D31"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:noFill/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="100"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
             <c:numRef>
-              <c:f>Summary_Results!$A$3:$A$22</c:f>
+              <c:f>Summary_Results!$AA$3:$AA$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1.67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>1.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>1.28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>1.63</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>1.22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>1.53</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>1.47</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>1.24</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>1.47</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>2.17</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16</c:v>
+                  <c:v>1.37</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17</c:v>
+                  <c:v>1.78</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>1.88</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19</c:v>
+                  <c:v>1.05</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>0.74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:srgbClr val="A5A5A5"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Summary_Results!$F$3:$F$22</c:f>
+              <c:f>Summary_Results!$AB$3:$AB$22</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.96</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:srgbClr val="FFC000"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="plus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="100"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary_Results!$AC$3:$AC$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.98</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.93</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.92</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:srgbClr val="4472C4"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:noFill/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary_Results!$AD$3:$AD$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.88</c:v>
+                  <c:v>2.13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.94</c:v>
+                  <c:v>2.4300000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.63</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0.96</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.94</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.95</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.97</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.98</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.01</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.99</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.92</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.04</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.94</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.95</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.93</c:v>
+                  <c:v>1.1599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.02</c:v>
+                  <c:v>1.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1214,11 +1497,12 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="319590688"/>
-        <c:axId val="319594216"/>
+        <c:overlap val="100"/>
+        <c:axId val="399350784"/>
+        <c:axId val="399342944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="319590688"/>
+        <c:axId val="399350784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1227,11 +1511,21 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
@@ -1240,13 +1534,73 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="319594216"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="399342944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1254,7 +1608,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319594216"/>
+        <c:axId val="399342944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -1262,15 +1616,38 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-NZ"/>
@@ -1279,25 +1656,108 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="319590688"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="399350784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
 </c:chartSpace>
 </file>
 
@@ -1326,11 +1786,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number from Biomedical in each group</a:t>
+              <a:t>Biomedical students in each group</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1495,11 +1956,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="324300240"/>
-        <c:axId val="324295928"/>
+        <c:axId val="511137368"/>
+        <c:axId val="511138544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324300240"/>
+        <c:axId val="511137368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1521,13 +1982,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324295928"/>
+        <c:crossAx val="511138544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1535,7 +1997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324295928"/>
+        <c:axId val="511138544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -1560,19 +2022,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324300240"/>
+        <c:crossAx val="511137368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1607,11 +2071,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number from EngSci in each group</a:t>
+              <a:t>Engsci students in each group</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1776,11 +2241,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="324299848"/>
-        <c:axId val="324288088"/>
+        <c:axId val="978058992"/>
+        <c:axId val="978059384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324299848"/>
+        <c:axId val="978058992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1802,13 +2267,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324288088"/>
+        <c:crossAx val="978059384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1816,7 +2282,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324288088"/>
+        <c:axId val="978059384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -1841,19 +2307,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324299848"/>
+        <c:crossAx val="978058992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1888,11 +2356,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number of European in each group</a:t>
+              <a:t>European students in each group</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2057,11 +2526,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="324291616"/>
-        <c:axId val="324292008"/>
+        <c:axId val="1135444328"/>
+        <c:axId val="1135435312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324291616"/>
+        <c:axId val="1135444328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2083,13 +2552,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324292008"/>
+        <c:crossAx val="1135435312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2097,7 +2567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324292008"/>
+        <c:axId val="1135435312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -2122,19 +2592,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324291616"/>
+        <c:crossAx val="1135444328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2169,11 +2641,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number of Pacific in each group</a:t>
+              <a:t>Pacific students in each group</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2338,11 +2811,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="324292400"/>
-        <c:axId val="324297104"/>
+        <c:axId val="399351176"/>
+        <c:axId val="399346472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324292400"/>
+        <c:axId val="399351176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2364,13 +2837,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324297104"/>
+        <c:crossAx val="399346472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2378,7 +2852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324297104"/>
+        <c:axId val="399346472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -2403,19 +2877,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324292400"/>
+        <c:crossAx val="399351176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2450,11 +2926,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number of Indian in each group</a:t>
+              <a:t>Indian students in each group</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2619,11 +3096,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="324293576"/>
-        <c:axId val="324294360"/>
+        <c:axId val="1129756384"/>
+        <c:axId val="1129761480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324293576"/>
+        <c:axId val="1129756384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2645,13 +3122,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324294360"/>
+        <c:crossAx val="1129761480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2659,7 +3137,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324294360"/>
+        <c:axId val="1129761480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -2684,19 +3162,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324293576"/>
+        <c:crossAx val="1129756384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2731,11 +3211,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number of Asian in each group</a:t>
+              <a:t>Asian students in each group</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2900,11 +3381,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="324303376"/>
-        <c:axId val="324302200"/>
+        <c:axId val="511102480"/>
+        <c:axId val="511103656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324303376"/>
+        <c:axId val="511102480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2926,13 +3407,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324302200"/>
+        <c:crossAx val="511103656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2940,7 +3422,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324302200"/>
+        <c:axId val="511103656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -2965,19 +3447,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324303376"/>
+        <c:crossAx val="511102480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3017,6 +3501,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3327,11 +3812,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="319596176"/>
-        <c:axId val="319595392"/>
+        <c:axId val="887083744"/>
+        <c:axId val="887074336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="319596176"/>
+        <c:axId val="887083744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3353,13 +3838,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="319595392"/>
+        <c:crossAx val="887074336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3367,7 +3853,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319595392"/>
+        <c:axId val="887074336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -3392,19 +3878,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="319596176"/>
+        <c:crossAx val="887083744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3439,11 +3927,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number from Civil in each group</a:t>
+              <a:t>Civil students in each group</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3608,11 +4097,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="319593824"/>
-        <c:axId val="319594608"/>
+        <c:axId val="399332360"/>
+        <c:axId val="399330400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="319593824"/>
+        <c:axId val="399332360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3634,13 +4123,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="319594608"/>
+        <c:crossAx val="399330400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3648,7 +4138,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319594608"/>
+        <c:axId val="399330400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -3673,19 +4163,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="319593824"/>
+        <c:crossAx val="399332360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3720,11 +4212,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number from Electrical in each group</a:t>
+              <a:t>Electrical students in each group</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3889,11 +4382,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="319595784"/>
-        <c:axId val="324288872"/>
+        <c:axId val="399346864"/>
+        <c:axId val="399347256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="319595784"/>
+        <c:axId val="399346864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3915,13 +4408,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324288872"/>
+        <c:crossAx val="399347256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3929,7 +4423,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324288872"/>
+        <c:axId val="399347256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -3954,19 +4448,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="319595784"/>
+        <c:crossAx val="399346864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4001,11 +4497,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number from CompSys in each group</a:t>
+              <a:t>Compsys students in each group</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4170,11 +4667,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="324294752"/>
-        <c:axId val="324298280"/>
+        <c:axId val="970825064"/>
+        <c:axId val="970818400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324294752"/>
+        <c:axId val="970825064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4196,13 +4693,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324298280"/>
+        <c:crossAx val="970818400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4210,7 +4708,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324298280"/>
+        <c:axId val="970818400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -4235,19 +4733,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324294752"/>
+        <c:crossAx val="970825064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4282,11 +4782,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number from Software in each group</a:t>
+              <a:t>Software students in each group</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4451,11 +4952,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="324290048"/>
-        <c:axId val="324290440"/>
+        <c:axId val="970823104"/>
+        <c:axId val="970827416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324290048"/>
+        <c:axId val="970823104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4477,13 +4978,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324290440"/>
+        <c:crossAx val="970827416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4491,7 +4993,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324290440"/>
+        <c:axId val="970827416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -4516,19 +5018,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324290048"/>
+        <c:crossAx val="970823104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4563,11 +5067,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number from Mechatronics in each group</a:t>
+              <a:t>Mechatronics students in each group</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4732,11 +5237,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="324289264"/>
-        <c:axId val="324299064"/>
+        <c:axId val="970822712"/>
+        <c:axId val="970823888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324289264"/>
+        <c:axId val="970822712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4758,13 +5263,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324299064"/>
+        <c:crossAx val="970823888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4772,7 +5278,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324299064"/>
+        <c:axId val="970823888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -4797,19 +5303,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324289264"/>
+        <c:crossAx val="970822712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4844,11 +5352,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number from Chemmat in each group</a:t>
+              <a:t>Chemmat students in each group</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5013,11 +5522,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="324295144"/>
-        <c:axId val="324293968"/>
+        <c:axId val="978065656"/>
+        <c:axId val="978060560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324295144"/>
+        <c:axId val="978065656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5039,13 +5548,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324293968"/>
+        <c:crossAx val="978060560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5053,7 +5563,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324293968"/>
+        <c:axId val="978060560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -5078,19 +5588,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324295144"/>
+        <c:crossAx val="978065656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5125,11 +5637,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number from Mechanical in each group</a:t>
+              <a:t>Mechanical students in each group</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5294,11 +5807,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="324297888"/>
-        <c:axId val="324289656"/>
+        <c:axId val="978057032"/>
+        <c:axId val="978064088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324297888"/>
+        <c:axId val="978057032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5320,13 +5833,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324289656"/>
+        <c:crossAx val="978064088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5334,7 +5848,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324289656"/>
+        <c:axId val="978064088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -5359,19 +5873,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="324297888"/>
+        <c:crossAx val="978057032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5379,6 +5895,551 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6731,7 +7792,7 @@
   </sheetPr>
   <dimension ref="A1:AF81"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="R49" sqref="R49"/>
     </sheetView>
   </sheetViews>
@@ -7521,8 +8582,8 @@
   </sheetPr>
   <dimension ref="A1:AF686"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23540,7 +24601,7 @@
   <sheetPr codeName="Sheet7">
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:AD22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
@@ -23565,10 +24626,22 @@
     <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="43" width="12.7109375" customWidth="1"/>
+    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="34" width="12" bestFit="1" customWidth="1"/>
+    <col min="35" max="43" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>2</v>
       </c>
@@ -23626,8 +24699,38 @@
       <c r="S1" s="30" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1" t="s">
+        <v>86</v>
+      </c>
+      <c r="W1" t="s">
+        <v>87</v>
+      </c>
+      <c r="X1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>67</v>
       </c>
@@ -23686,7 +24789,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="34">
         <v>1</v>
       </c>
@@ -23744,8 +24847,38 @@
       <c r="S3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U3">
+        <v>2.89</v>
+      </c>
+      <c r="V3">
+        <v>4.25</v>
+      </c>
+      <c r="W3">
+        <v>4.72</v>
+      </c>
+      <c r="X3">
+        <v>5.71</v>
+      </c>
+      <c r="Y3">
+        <v>7.17</v>
+      </c>
+      <c r="Z3">
+        <v>2.89</v>
+      </c>
+      <c r="AA3">
+        <v>1.36</v>
+      </c>
+      <c r="AB3">
+        <v>0.47</v>
+      </c>
+      <c r="AC3">
+        <v>0.98</v>
+      </c>
+      <c r="AD3">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
         <v>2</v>
       </c>
@@ -23803,8 +24936,38 @@
       <c r="S4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <v>2.63</v>
+      </c>
+      <c r="V4">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="W4">
+        <v>4.88</v>
+      </c>
+      <c r="X4">
+        <v>5.85</v>
+      </c>
+      <c r="Y4">
+        <v>6.81</v>
+      </c>
+      <c r="Z4">
+        <v>2.63</v>
+      </c>
+      <c r="AA4">
+        <v>1.67</v>
+      </c>
+      <c r="AB4">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AC4">
+        <v>0.97</v>
+      </c>
+      <c r="AD4">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="34">
         <v>3</v>
       </c>
@@ -23862,8 +25025,38 @@
       <c r="S5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <v>2.94</v>
+      </c>
+      <c r="V5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="W5">
+        <v>5.33</v>
+      </c>
+      <c r="X5">
+        <v>5.84</v>
+      </c>
+      <c r="Y5">
+        <v>6.27</v>
+      </c>
+      <c r="Z5">
+        <v>2.94</v>
+      </c>
+      <c r="AA5">
+        <v>1.45</v>
+      </c>
+      <c r="AB5">
+        <v>0.94</v>
+      </c>
+      <c r="AC5">
+        <v>0.51</v>
+      </c>
+      <c r="AD5">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="34">
         <v>4</v>
       </c>
@@ -23921,8 +25114,38 @@
       <c r="S6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <v>2.58</v>
+      </c>
+      <c r="V6">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="W6">
+        <v>4.93</v>
+      </c>
+      <c r="X6">
+        <v>5.39</v>
+      </c>
+      <c r="Y6">
+        <v>7.52</v>
+      </c>
+      <c r="Z6">
+        <v>2.58</v>
+      </c>
+      <c r="AA6">
+        <v>1.98</v>
+      </c>
+      <c r="AB6">
+        <v>0.37</v>
+      </c>
+      <c r="AC6">
+        <v>0.46</v>
+      </c>
+      <c r="AD6">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="34">
         <v>5</v>
       </c>
@@ -23980,8 +25203,38 @@
       <c r="S7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <v>3.25</v>
+      </c>
+      <c r="V7">
+        <v>4.53</v>
+      </c>
+      <c r="W7">
+        <v>5</v>
+      </c>
+      <c r="X7">
+        <v>5.57</v>
+      </c>
+      <c r="Y7">
+        <v>8.01</v>
+      </c>
+      <c r="Z7">
+        <v>3.25</v>
+      </c>
+      <c r="AA7">
+        <v>1.28</v>
+      </c>
+      <c r="AB7">
+        <v>0.47</v>
+      </c>
+      <c r="AC7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AD7">
+        <v>2.4300000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="34">
         <v>6</v>
       </c>
@@ -24039,8 +25292,38 @@
       <c r="S8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <v>3.55</v>
+      </c>
+      <c r="V8">
+        <v>4.22</v>
+      </c>
+      <c r="W8">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="X8">
+        <v>5.79</v>
+      </c>
+      <c r="Y8">
+        <v>7.39</v>
+      </c>
+      <c r="Z8">
+        <v>3.55</v>
+      </c>
+      <c r="AA8">
+        <v>0.67</v>
+      </c>
+      <c r="AB8">
+        <v>0.89</v>
+      </c>
+      <c r="AC8">
+        <v>0.68</v>
+      </c>
+      <c r="AD8">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="34">
         <v>7</v>
       </c>
@@ -24098,8 +25381,38 @@
       <c r="S9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <v>2.83</v>
+      </c>
+      <c r="V9">
+        <v>4.46</v>
+      </c>
+      <c r="W9">
+        <v>5.13</v>
+      </c>
+      <c r="X9">
+        <v>5.58</v>
+      </c>
+      <c r="Y9">
+        <v>6.88</v>
+      </c>
+      <c r="Z9">
+        <v>2.83</v>
+      </c>
+      <c r="AA9">
+        <v>1.63</v>
+      </c>
+      <c r="AB9">
+        <v>0.67</v>
+      </c>
+      <c r="AC9">
+        <v>0.45</v>
+      </c>
+      <c r="AD9">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="34">
         <v>8</v>
       </c>
@@ -24157,8 +25470,38 @@
       <c r="S10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <v>3.25</v>
+      </c>
+      <c r="V10">
+        <v>4.47</v>
+      </c>
+      <c r="W10">
+        <v>5.21</v>
+      </c>
+      <c r="X10">
+        <v>5.59</v>
+      </c>
+      <c r="Y10">
+        <v>7.07</v>
+      </c>
+      <c r="Z10">
+        <v>3.25</v>
+      </c>
+      <c r="AA10">
+        <v>1.22</v>
+      </c>
+      <c r="AB10">
+        <v>0.74</v>
+      </c>
+      <c r="AC10">
+        <v>0.38</v>
+      </c>
+      <c r="AD10">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="34">
         <v>9</v>
       </c>
@@ -24216,8 +25559,38 @@
       <c r="S11">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <v>1.9</v>
+      </c>
+      <c r="V11">
+        <v>4.7</v>
+      </c>
+      <c r="W11">
+        <v>5.19</v>
+      </c>
+      <c r="X11">
+        <v>5.7</v>
+      </c>
+      <c r="Y11">
+        <v>6.79</v>
+      </c>
+      <c r="Z11">
+        <v>1.9</v>
+      </c>
+      <c r="AA11">
+        <v>2.8</v>
+      </c>
+      <c r="AB11">
+        <v>0.49</v>
+      </c>
+      <c r="AC11">
+        <v>0.51</v>
+      </c>
+      <c r="AD11">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="34">
         <v>10</v>
       </c>
@@ -24275,8 +25648,38 @@
       <c r="S12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <v>2.98</v>
+      </c>
+      <c r="V12">
+        <v>4.51</v>
+      </c>
+      <c r="W12">
+        <v>4.95</v>
+      </c>
+      <c r="X12">
+        <v>5.52</v>
+      </c>
+      <c r="Y12">
+        <v>7.31</v>
+      </c>
+      <c r="Z12">
+        <v>2.98</v>
+      </c>
+      <c r="AA12">
+        <v>1.53</v>
+      </c>
+      <c r="AB12">
+        <v>0.44</v>
+      </c>
+      <c r="AC12">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AD12">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="34">
         <v>11</v>
       </c>
@@ -24334,8 +25737,38 @@
       <c r="S13">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <v>2.78</v>
+      </c>
+      <c r="V13">
+        <v>4.26</v>
+      </c>
+      <c r="W13">
+        <v>5.21</v>
+      </c>
+      <c r="X13">
+        <v>5.76</v>
+      </c>
+      <c r="Y13">
+        <v>6.98</v>
+      </c>
+      <c r="Z13">
+        <v>2.78</v>
+      </c>
+      <c r="AA13">
+        <v>1.47</v>
+      </c>
+      <c r="AB13">
+        <v>0.96</v>
+      </c>
+      <c r="AC13">
+        <v>0.54</v>
+      </c>
+      <c r="AD13">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="34">
         <v>12</v>
       </c>
@@ -24393,8 +25826,38 @@
       <c r="S14">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U14">
+        <v>3.23</v>
+      </c>
+      <c r="V14">
+        <v>4.47</v>
+      </c>
+      <c r="W14">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="X14">
+        <v>5.91</v>
+      </c>
+      <c r="Y14">
+        <v>6.74</v>
+      </c>
+      <c r="Z14">
+        <v>3.23</v>
+      </c>
+      <c r="AA14">
+        <v>1.24</v>
+      </c>
+      <c r="AB14">
+        <v>0.42</v>
+      </c>
+      <c r="AC14">
+        <v>1.02</v>
+      </c>
+      <c r="AD14">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="34">
         <v>13</v>
       </c>
@@ -24452,8 +25915,38 @@
       <c r="S15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <v>3.1</v>
+      </c>
+      <c r="V15">
+        <v>4.57</v>
+      </c>
+      <c r="W15">
+        <v>4.82</v>
+      </c>
+      <c r="X15">
+        <v>5.8</v>
+      </c>
+      <c r="Y15">
+        <v>7.72</v>
+      </c>
+      <c r="Z15">
+        <v>3.1</v>
+      </c>
+      <c r="AA15">
+        <v>1.47</v>
+      </c>
+      <c r="AB15">
+        <v>0.25</v>
+      </c>
+      <c r="AC15">
+        <v>0.97</v>
+      </c>
+      <c r="AD15">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="34">
         <v>14</v>
       </c>
@@ -24511,8 +26004,38 @@
       <c r="S16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <v>3.56</v>
+      </c>
+      <c r="V16">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="W16">
+        <v>5.18</v>
+      </c>
+      <c r="X16">
+        <v>5.84</v>
+      </c>
+      <c r="Y16">
+        <v>7.47</v>
+      </c>
+      <c r="Z16">
+        <v>3.56</v>
+      </c>
+      <c r="AA16">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AB16">
+        <v>1.06</v>
+      </c>
+      <c r="AC16">
+        <v>0.66</v>
+      </c>
+      <c r="AD16">
+        <v>1.63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="34">
         <v>15</v>
       </c>
@@ -24570,8 +26093,38 @@
       <c r="S17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U17">
+        <v>2.31</v>
+      </c>
+      <c r="V17">
+        <v>4.47</v>
+      </c>
+      <c r="W17">
+        <v>5.14</v>
+      </c>
+      <c r="X17">
+        <v>5.83</v>
+      </c>
+      <c r="Y17">
+        <v>6.55</v>
+      </c>
+      <c r="Z17">
+        <v>2.31</v>
+      </c>
+      <c r="AA17">
+        <v>2.17</v>
+      </c>
+      <c r="AB17">
+        <v>0.66</v>
+      </c>
+      <c r="AC17">
+        <v>0.7</v>
+      </c>
+      <c r="AD17">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="34">
         <v>16</v>
       </c>
@@ -24629,8 +26182,38 @@
       <c r="S18">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <v>3.08</v>
+      </c>
+      <c r="V18">
+        <v>4.45</v>
+      </c>
+      <c r="W18">
+        <v>4.72</v>
+      </c>
+      <c r="X18">
+        <v>5.6</v>
+      </c>
+      <c r="Y18">
+        <v>7.7</v>
+      </c>
+      <c r="Z18">
+        <v>3.08</v>
+      </c>
+      <c r="AA18">
+        <v>1.37</v>
+      </c>
+      <c r="AB18">
+        <v>0.27</v>
+      </c>
+      <c r="AC18">
+        <v>0.88</v>
+      </c>
+      <c r="AD18">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="34">
         <v>17</v>
       </c>
@@ -24688,8 +26271,38 @@
       <c r="S19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U19">
+        <v>2.74</v>
+      </c>
+      <c r="V19">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="W19">
+        <v>5.05</v>
+      </c>
+      <c r="X19">
+        <v>5.65</v>
+      </c>
+      <c r="Y19">
+        <v>6.9</v>
+      </c>
+      <c r="Z19">
+        <v>2.74</v>
+      </c>
+      <c r="AA19">
+        <v>1.78</v>
+      </c>
+      <c r="AB19">
+        <v>0.53</v>
+      </c>
+      <c r="AC19">
+        <v>0.59</v>
+      </c>
+      <c r="AD19">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="34">
         <v>18</v>
       </c>
@@ -24747,8 +26360,38 @@
       <c r="S20">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <v>2.56</v>
+      </c>
+      <c r="V20">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="W20">
+        <v>5.23</v>
+      </c>
+      <c r="X20">
+        <v>5.74</v>
+      </c>
+      <c r="Y20">
+        <v>6.7</v>
+      </c>
+      <c r="Z20">
+        <v>2.56</v>
+      </c>
+      <c r="AA20">
+        <v>1.88</v>
+      </c>
+      <c r="AB20">
+        <v>0.79</v>
+      </c>
+      <c r="AC20">
+        <v>0.52</v>
+      </c>
+      <c r="AD20">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="34">
         <v>19</v>
       </c>
@@ -24806,8 +26449,38 @@
       <c r="S21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U21">
+        <v>3.23</v>
+      </c>
+      <c r="V21">
+        <v>4.28</v>
+      </c>
+      <c r="W21">
+        <v>4.82</v>
+      </c>
+      <c r="X21">
+        <v>5.74</v>
+      </c>
+      <c r="Y21">
+        <v>6.91</v>
+      </c>
+      <c r="Z21">
+        <v>3.23</v>
+      </c>
+      <c r="AA21">
+        <v>1.05</v>
+      </c>
+      <c r="AB21">
+        <v>0.54</v>
+      </c>
+      <c r="AC21">
+        <v>0.92</v>
+      </c>
+      <c r="AD21">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="34">
         <v>20</v>
       </c>
@@ -24864,6 +26537,36 @@
       </c>
       <c r="S22">
         <v>6</v>
+      </c>
+      <c r="U22">
+        <v>3.4</v>
+      </c>
+      <c r="V22">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="W22">
+        <v>5.2</v>
+      </c>
+      <c r="X22">
+        <v>5.67</v>
+      </c>
+      <c r="Y22">
+        <v>7.06</v>
+      </c>
+      <c r="Z22">
+        <v>3.4</v>
+      </c>
+      <c r="AA22">
+        <v>0.74</v>
+      </c>
+      <c r="AB22">
+        <v>1.06</v>
+      </c>
+      <c r="AC22">
+        <v>0.48</v>
+      </c>
+      <c r="AD22">
+        <v>1.39</v>
       </c>
     </row>
   </sheetData>
@@ -24877,7 +26580,7 @@
     <StoredFile>
       <FileName>Untitled</FileName>
       <LanguageName>PuLP</LanguageName>
-      <ModelPaneVisible>true</ModelPaneVisible>
+      <ModelPaneVisible>false</ModelPaneVisible>
       <ModelSettings/>
       <FileText># ============================================================================
 # Group Allocator - allocates students to balanced groups
@@ -24885,14 +26588,14 @@
 # The MIT License (MIT)
 # Copyright (c) 2014 Michael Fairley (mfai035@aucklanduni.ac.nz)
 # Permission is hereby granted, free of charge, to any person obtaining a copy of
-# this software and associated documentation files (the "Software"), to deal in
+# this software and associated documentation files (the 'Software'), to deal in
 # the Software without restriction, including without limitation the rights to
 # use, copy, modify, merge, publish, distribute, sublicense, and/or sell copies of
 # the Software, and to permit persons to whom the Software is furnished to do so,
 # subject to the following conditions:
 # The above copyright notice and this permission notice shall be included in all
 # copies or substantial portions of the Software.
-# THE SOFTWARE IS PROVIDED "AS IS", WITHOUT WARRANTY OF ANY KIND, EXPRESS OR
+# THE SOFTWARE IS PROVIDED 'AS IS', WITHOUT WARRANTY OF ANY KIND, EXPRESS OR
 # IMPLIED, INCLUDING BUT NOT LIMITED TO THE WARRANTIES OF MERCHANTABILITY, FITNESS
 # FOR A PARTICULAR PURPOSE AND NONINFRINGEMENT. IN NO EVENT SHALL THE AUTHORS OR
 # COPYRIGHT HOLDERS BE LIABLE FOR ANY CLAIM, DAMAGES OR OTHER LIABILITY, WHETHER
@@ -24905,6 +26608,7 @@
 #
 # ============================================================================
 from pulp import *
+from System import Array
 import datetime
 problem = LpProblem('ENGGEN403', LpMinimize)
 print('Creating model...')
@@ -25213,12 +26917,51 @@
     for e in ETHNICITIES:
         col_index += 1
         ws.Cells(cell_index, col_index).Value = ethnicities_group[e][g]
+# Insert data for box plots
+col_index += 1
+ws.Cells(1, col_index + 1).Value = 'gpa_min'
+ws.Cells(1, col_index + 2).Value = 'gpa_q1'
+ws.Cells(1, col_index + 3).Value = 'gpa_median'
+ws.Cells(1, col_index + 4).Value = 'gpa_q3'
+ws.Cells(1, col_index + 5).Value = 'gpa_max'
+ws.Cells(1, col_index + 6).Value = 'gpa_d_min'
+ws.Cells(1, col_index + 7).Value = 'gpa_d_q1'
+ws.Cells(1, col_index + 8).Value = 'gpa_d_median'
+ws.Cells(1, col_index + 9).Value = 'gpa_d_q3'
+ws.Cells(1, col_index + 10).Value = 'gpa_d_max'
+# Create array for each group containing gpas
+data_summary = {}
+for g in GROUPS:
+    array = Array.CreateInstance(object, len(students_in_group[g]))
+    for i in range(len(students_in_group[g])):
+        student = students_in_group[g][i]
+        array[i] = gpa[student]
+    min_gpa = Application.WorksheetFunction.Min(array)
+    q1_gpa = Application.WorksheetFunction.Quartile(array, 1)
+    med_gpa = Application.WorksheetFunction.Median(array)
+    q3_gpa = Application.WorksheetFunction.Quartile(array, 3)
+    max_gpa = Application.WorksheetFunction.Max(array)
+    data_summary[g] = [min_gpa, q1_gpa, med_gpa, q3_gpa, max_gpa]
+row_index = 2
+for g in GROUPS:
+    row_index += 1
+    ws.Cells(row_index, col_index + 1).Value = '%.2f' % data_summary[g][0]
+    ws.Cells(row_index, col_index + 2).Value = '%.2f' % data_summary[g][1]
+    ws.Cells(row_index, col_index + 3).Value = '%.2f' % data_summary[g][2]
+    ws.Cells(row_index, col_index + 4).Value = '%.2f' % data_summary[g][3]
+    ws.Cells(row_index, col_index + 5).Value = '%.2f' % data_summary[g][4]
+    # Differences needed for charting
+    ws.Cells(row_index, col_index + 6).Value = '%.2f' % data_summary[g][0]
+    ws.Cells(row_index, col_index + 7).Value = '%.2f' % (data_summary[g][1] -  data_summary[g][0])
+    ws.Cells(row_index, col_index + 8).Value = '%.2f' % (data_summary[g][2] -  data_summary[g][1])
+    ws.Cells(row_index, col_index + 9).Value = '%.2f' % (data_summary[g][3] -  data_summary[g][2])
+    ws.Cells(row_index, col_index + 10).Value = '%.2f' % (data_summary[g][4] -  data_summary[g][3])
 # Autofit columns in Summary_Results
 ws.Activate()
 ws.Cells.Select()
 Application.Selection.Columns.AutoFit()
-ws.Range(ws.Cells(2, 5), ws.Cells(number_groups+2, 6)).NumberFormat = "0.00"
-ws.Range(ws.Cells(2, 1), ws.Cells(2, 6 + len(SPECIALISATIONS) + len(ETHNICITIES))).Style = "Good"
+ws.Range(ws.Cells(2, 5), ws.Cells(number_groups+2, 6)).NumberFormat = '0.00'
+ws.Range(ws.Cells(2, 1), ws.Cells(2, 6 + len(SPECIALISATIONS) + len(ETHNICITIES))).Style = 'Good'
 ws.Range(ws.cells(1, 1), ws.Cells(number_groups+2, 1)).Borders(10).LineStyle = 1
 ws.Range(ws.cells(1, 1), ws.Cells(number_groups+2, 1)).HorizontalAlignment = -4131
 ws.Cells(number_groups+5, 1).Select()
@@ -25230,34 +26973,77 @@
         Application.DisplayAlerts = False
         sheet.Delete()
         Application.DisplayAlerts = True
-x_axis_range = ws.Range(ws.Cells(3, 1), ws.Cells(2 + number_groups, 1))
-# GPA mean and variance graph
+# GPA Box Plot Chart
+# Select data range
 print('Charting GPA . . .')
-Application.Worksheets('Summary_Results').Activate()
-ws.Cells(number_groups+5, 1).Select()
-Application.Worksheets('Summary_Results').Shapes.AddChart(201, 54).Select()
+ws.Range(ws.Cells(3, col_index + 6), ws.Cells(2 + number_groups, col_index + 10)).Select()
+Application.Worksheets('Summary_Results').Shapes.AddChart2(297, 52).Select()
 a = Application.ActiveChart
-a.SeriesCollection().NewSeries()
-a.FullSeriesCollection(1).Name = "GPA"
-a.FullSeriesCollection(1).Values = ws.Range(ws.Cells(3, 5), ws.Cells(2 + number_groups, 5))
-a.FullSeriesCollection(1).XValues = x_axis_range
-a.SeriesCollection().NewSeries()
-a.FullSeriesCollection(2).Name = "GPA Variance"
-a.FullSeriesCollection(2).Values = ws.Range(ws.Cells(3, 6), ws.Cells(2 + number_groups, 6))
-a.FullSeriesCollection(2).XValues = x_axis_range
+a.FullSeriesCollection(1).Select()
+Application.Selection.Format.Fill.Visible = 0
+Application.Selection.Format.Line.Visible = 0
+a.FullSeriesCollection(2).Select()
+Application.Selection.Format.Fill.Visible = 0
+Application.Selection.Format.Line.Visible = 0
+a.FullSeriesCollection(2).HasErrorBars = True
+#a.FullSeriesCollection(2).ErrorBars.Select()
+a.FullSeriesCollection(2).ErrorBar(Direction=1, Include=3, Type=2, Amount=100)
+a.FullSeriesCollection(5).Select()
+Application.Selection.Format.Fill.Visible = 0
+Application.Selection.Format.Line.Visible = 0
+a.FullSeriesCollection(4).HasErrorBars = True
+a.FullSeriesCollection(4).ErrorBar(Direction=1, Include=2, Type=2, Amount=100)
+a.FullSeriesCollection(4).Select()
+Application.Selection.Format.Fill.Visible = 0
+Application.Selection.Format.Line.Visible = 1
+Application.Selection.Format.Line.ForeColor.ObjectThemeColor = 13
+a.FullSeriesCollection(3).Select()
+Application.Selection.Format.Fill.Visible = 0
+Application.Selection.Format.Line.Visible = 1
+Application.Selection.Format.Line.ForeColor.ObjectThemeColor = 13
 a.SetElement(2)
 a.SetElement(306)
 a.SetElement(301)
 a.SetElement(102)
-a.ChartTitle.Text = "Mean GPA and Variance of GPA"
+a.Legend.Select()
+Application.Selection.Delete()
+a.ChartTitle.Text = 'GPA spread per group (lines bottom to top = Min, Q1, Median, Q3, Max)'
 a.Axes(1, 1).HasTitle = True
-a.Axes(1, 1).AxisTitle.Text = "Group"
+a.Axes(1, 1).AxisTitle.Text = 'Group'
 a.Axes(2, 1).HasTitle = True
-a.Axes(2, 1).AxisTitle.Text = "GPA"
+a.Axes(2, 1).AxisTitle.Text = 'GPA'
 a.Axes(2).MaximumScale = 9
 a.Axes(2).MinimumScale = 0
-a.Location(Where=1, Name="GPA_Chart")
+a.Location(Where=1, Name='GPA_Chart')
 a.deselect()
+# GPA mean and variance graph
+# print('Charting GPA . . .')
+# Application.Worksheets('Summary_Results').Activate()
+# ws.Cells(number_groups+5, 1).Select()
+# Application.Worksheets('Summary_Results').Shapes.AddChart(201, 54).Select()
+# a = Application.ActiveChart
+# a.SeriesCollection().NewSeries()
+# a.FullSeriesCollection(1).Name = 'GPA'
+# a.FullSeriesCollection(1).Values = ws.Range(ws.Cells(3, 5), ws.Cells(2 + number_groups, 5))
+# a.FullSeriesCollection(1).XValues = x_axis_range
+# a.SeriesCollection().NewSeries()
+# a.FullSeriesCollection(2).Name = 'GPA Variance'
+# a.FullSeriesCollection(2).Values = ws.Range(ws.Cells(3, 6), ws.Cells(2 + number_groups, 6))
+# a.FullSeriesCollection(2).XValues = x_axis_range
+# a.SetElement(2)
+# a.SetElement(306)
+# a.SetElement(301)
+# a.SetElement(102)
+# a.ChartTitle.Text = 'Mean GPA and Variance of GPA'
+# a.Axes(1, 1).HasTitle = True
+# a.Axes(1, 1).AxisTitle.Text = 'Group'
+# a.Axes(2, 1).HasTitle = True
+# a.Axes(2, 1).AxisTitle.Text = 'GPA'
+# a.Axes(2).MaximumScale = 9
+# a.Axes(2).MinimumScale = 0
+# a.Location(Where=1, Name='GPA_Chart')
+# a.deselect()
+x_axis_range = ws.Range(ws.Cells(3, 1), ws.Cells(2 + number_groups, 1))
 # Gender
 print('Charting Gender . . .')
 Application.Worksheets('Summary_Results').Activate()
@@ -25265,25 +27051,25 @@
 Application.Worksheets('Summary_Results').Shapes.AddChart(201, 54).Select()
 a = Application.ActiveChart
 a.SeriesCollection().NewSeries()
-a.FullSeriesCollection(1).Name = "Male"
+a.FullSeriesCollection(1).Name = 'Male'
 a.FullSeriesCollection(1).Values = ws.Range(ws.Cells(3, 3), ws.Cells(2 + number_groups, 3))
 a.FullSeriesCollection(1).XValues = x_axis_range
 a.SeriesCollection().NewSeries()
-a.FullSeriesCollection(2).Name = "Female"
+a.FullSeriesCollection(2).Name = 'Female'
 a.FullSeriesCollection(2).Values = ws.Range(ws.Cells(3, 4), ws.Cells(2 + number_groups, 4))
 a.FullSeriesCollection(2).XValues = x_axis_range
 a.SetElement(2)
 a.SetElement(306)
 a.SetElement(301)
 a.SetElement(102)
-a.ChartTitle.Text = "Number of Males and Females in each group"
+a.ChartTitle.Text = 'Number of Males and Females in each group'
 a.Axes(1, 1).HasTitle = True
-a.Axes(1, 1).AxisTitle.Text = "Group"
+a.Axes(1, 1).AxisTitle.Text = 'Group'
 a.Axes(2, 1).HasTitle = True
-a.Axes(2, 1).AxisTitle.Text = "Number of Students"
+a.Axes(2, 1).AxisTitle.Text = 'Number of Students'
 a.Axes(2).MaximumScale = m2 + 1
 a.Axes(2).MinimumScale = 0
-a.Location(Where=1, Name="Gender_Chart")
+a.Location(Where=1, Name='Gender_Chart')
 a.deselect()
 # Specialisations
 print('Charting Specialisations . . .')
@@ -25305,14 +27091,14 @@
     a.SetElement(306)
     a.SetElement(301)
     a.SetElement(102)
-    a.ChartTitle.Text = "Number from %s in each group" % s
+    a.ChartTitle.Text = '%s students in each group' % s.title()
     a.Axes(1, 1).HasTitle = True
-    a.Axes(1, 1).AxisTitle.Text = "Group"
+    a.Axes(1, 1).AxisTitle.Text = 'Group'
     a.Axes(2, 1).HasTitle = True
-    a.Axes(2, 1).AxisTitle.Text = "Number of Students"
+    a.Axes(2, 1).AxisTitle.Text = 'Number of Students'
     a.Axes(2).MaximumScale = m2 + 1
     a.Axes(2).MinimumScale = 0
-    title = "%s_Chart" % s
+    title = '%s_Chart' % s
     a.Location(Where=1, Name=title)
     wb.Sheets(title).Tab.ThemeColor = 9
     wb.Sheets(title).Tab.TintAndShade = 0
@@ -25336,14 +27122,14 @@
     a.SetElement(306)
     a.SetElement(301)
     a.SetElement(102)
-    a.ChartTitle.Text = "Number of %s in each group" % e
+    a.ChartTitle.Text = '%s students in each group' % e.title()
     a.Axes(1, 1).HasTitle = True
-    a.Axes(1, 1).AxisTitle.Text = "Group"
+    a.Axes(1, 1).AxisTitle.Text = 'Group'
     a.Axes(2, 1).HasTitle = True
-    a.Axes(2, 1).AxisTitle.Text = "Number of Students"
+    a.Axes(2, 1).AxisTitle.Text = 'Number of Students'
     a.Axes(2).MaximumScale = m2 + 1
     a.Axes(2).MinimumScale = 0
-    title = "%s(E)_Chart" % e
+    title = '%s(E)_Chart' % e
     a.Location(Where=1, Name=title)
     wb.Sheets(title).Tab.ThemeColor = 6
     wb.Sheets(title).Tab.TintAndShade = 0
@@ -25395,7 +27181,7 @@
         ws.Cells(row_index, 4).Value = specialisation[s]
         ws.Cells(row_index, 5).Value = '%s@aucklanduni.ac.nz' % UPI[s]
         ws.Cells(row_index, 6).Value = '%.2f' % gpa[s]
-        ws.Range(ws.Cells(row_index, 6), ws.Cells(row_index, 6)).NumberFormat = "0.00"
+        ws.Range(ws.Cells(row_index, 6), ws.Cells(row_index, 6)).NumberFormat = '0.00'
         ws.Cells(row_index, 7).Value = ethnicity[s]
         # Space between each group
     row_index += 1
@@ -25443,14 +27229,14 @@
         ws.Cells(row_index, 4).Value = specialisation[s]
         ws.Cells(row_index, 5).Value = '%s@aucklanduni.ac.nz' % UPI[s]
         ws.Cells(row_index, 6).Value = '%.2f' % gpa[s]
-        ws.Range(ws.Cells(row_index, 6), ws.Cells(row_index, 6)).NumberFormat = "0.00"
+        ws.Range(ws.Cells(row_index, 6), ws.Cells(row_index, 6)).NumberFormat = '0.00'
         ws.Cells(row_index, 7).Value = ethnicity[s]
     # Mean GPA
     row_index += 2
     ws.Cells(row_index, 5).Value = 'Mean GPA'
     ws.Cells(row_index, 5).Font.Bold = True
     ws.Cells(row_index, 6).Value = '%.2f' % gpa_mean_group[g]
-    ws.Range(ws.Cells(row_index, 6), ws.Cells(row_index, 6)).NumberFormat = "0.00"
+    ws.Range(ws.Cells(row_index, 6), ws.Cells(row_index, 6)).NumberFormat = '0.00'
     # Activate and autofit
     ws.Activate()
     ws.Cells.Select()
@@ -25567,7 +27353,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AEB1B49-4359-4359-BC5B-4D866260A6AE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69B6A1AB-E3EC-452A-8098-015E174BC117}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://opensolver.org"/>

</xml_diff>